<commit_message>
Contacts Final Changes - 6th July 2023
</commit_message>
<xml_diff>
--- a/TestData/T2056_ContactDetailsPage_Activities_AddNewContact.xlsx
+++ b/TestData/T2056_ContactDetailsPage_Activities_AddNewContact.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngoyal0630\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6F1E17-5EC5-4A99-B5ED-EC983848E6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13440" windowHeight="2955" activeTab="1"/>
+    <workbookView xWindow="3624" yWindow="1500" windowWidth="19416" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -77,9 +78,6 @@
     <t>Conference 01</t>
   </si>
   <si>
-    <t>Nicole Bicho</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -105,12 +103,15 @@
   </si>
   <si>
     <t>ContactType</t>
+  </si>
+  <si>
+    <t>Drew Koecher</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,27 +435,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -464,25 +465,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +504,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -530,25 +531,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -559,33 +560,33 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" t="s">
         <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -595,24 +596,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>